<commit_message>
typo updates + test sheet updates
</commit_message>
<xml_diff>
--- a/solidity/Rules_Test_data.xlsx
+++ b/solidity/Rules_Test_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\eLearning\IITM_ACSE\Capstone\ACSECapstone_wip\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sghew\OneDrive\Documents\GitHub\ACSECapstone\solidity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EEC4B96-80FD-4193-89E8-368FB533AFD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50AE0C5B-27B0-4A48-9232-A1995A3E0ABD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57435" yWindow="-165" windowWidth="29130" windowHeight="15810" xr2:uid="{374E2EE5-8CBB-42A4-BB00-FF69D8D8B5B1}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{374E2EE5-8CBB-42A4-BB00-FF69D8D8B5B1}"/>
   </bookViews>
   <sheets>
     <sheet name="DOM-101" sheetId="1" r:id="rId1"/>
@@ -201,9 +201,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="171" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
-    <numFmt numFmtId="188" formatCode="0E+00"/>
-    <numFmt numFmtId="189" formatCode="[$-409]m/d/yy\ h:mm:ss\ AM/PM;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="165" formatCode="0E+00"/>
+    <numFmt numFmtId="166" formatCode="[$-409]m/d/yy\ h:mm:ss\ AM/PM;@"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -442,10 +442,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -456,15 +453,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="188" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -479,20 +473,26 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="189" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="189" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -834,33 +834,33 @@
       <c r="C1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="15">
+      <c r="D1" s="13">
         <v>60</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="13" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C2" s="16">
+      <c r="C2" s="14">
         <v>60</v>
       </c>
-      <c r="D2" s="17">
+      <c r="D2" s="15">
         <f>+D1*60</f>
         <v>3600</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="15" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="10" t="s">
         <v>28</v>
       </c>
       <c r="C3" s="2"/>
@@ -868,31 +868,31 @@
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="29" t="s">
+      <c r="E4" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="30" t="s">
+      <c r="G4" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="21" t="s">
+      <c r="H4" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="I4" s="21" t="s">
+      <c r="I4" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="J4" s="21" t="s">
+      <c r="J4" s="19" t="s">
         <v>34</v>
       </c>
     </row>
@@ -900,53 +900,53 @@
       <c r="B5" s="3">
         <v>101</v>
       </c>
-      <c r="C5" s="32" t="str">
+      <c r="C5" s="28" t="str">
         <f>_xlfn.CONCAT("D",B5)</f>
         <v>D101</v>
       </c>
-      <c r="D5" s="33">
+      <c r="D5" s="29">
         <v>45207.385416666664</v>
       </c>
       <c r="E5" s="2">
         <v>2</v>
       </c>
-      <c r="F5" s="33">
+      <c r="F5" s="29">
         <f>D5+E5/24</f>
         <v>45207.46875</v>
       </c>
-      <c r="G5" s="20">
+      <c r="G5" s="18">
         <v>10</v>
       </c>
-      <c r="H5" s="28" t="s">
+      <c r="H5" s="24" t="s">
         <v>13</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>35</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="31" t="str">
+      <c r="B6" s="27" t="str">
         <f>_xlfn.CONCAT(B5,",",C5,",",D6,",",F6,",",I5,",",J5)</f>
-        <v>101,D101,1696756500,1696763700,BOM,NYC</v>
-      </c>
-      <c r="C6" s="18" t="s">
+        <v>101,D101,1696756500,1696763700,BOM,DEL</v>
+      </c>
+      <c r="C6" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="17">
         <f>(D5-25569)*86400</f>
         <v>1696756499.9999998</v>
       </c>
-      <c r="F6" s="19">
+      <c r="F6" s="17">
         <f>(F5-25569)*86400</f>
         <v>1696763700</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="12">
         <f>G5*1000000000000000000</f>
         <v>1E+19</v>
       </c>
@@ -955,14 +955,14 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="34">
+      <c r="D7" s="30">
         <f>(D6/86400)+DATE(1970,1,1)</f>
         <v>45207.385416666664</v>
       </c>
-      <c r="F7" s="34">
+      <c r="F7" s="30">
         <f>(F6/86400)+DATE(1970,1,1)</f>
         <v>45207.46875</v>
       </c>
@@ -973,76 +973,76 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="D10" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="26"/>
-      <c r="F10" s="5" t="s">
+      <c r="E10" s="32"/>
+      <c r="F10" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5" t="s">
+      <c r="G10" s="33"/>
+      <c r="H10" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="I10" s="5"/>
+      <c r="I10" s="33"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B11" s="10"/>
-      <c r="C11" s="7" t="s">
+      <c r="B11" s="34"/>
+      <c r="C11" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="24" t="s">
+      <c r="D11" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="23" t="s">
+      <c r="E11" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="I11" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="7">
         <v>1</v>
       </c>
-      <c r="D12" s="27" t="s">
+      <c r="D12" s="23" t="s">
         <v>26</v>
       </c>
       <c r="E12" s="3">
         <f>$D$6-(24*($C$2))</f>
         <v>1696755059.9999998</v>
       </c>
-      <c r="F12" s="34" t="str">
+      <c r="F12" s="30" t="str">
         <f>IFERROR((D12/86400)+DATE(1970,1,1),_xlfn.CONCAT("Before ==&gt;"))</f>
         <v>Before ==&gt;</v>
       </c>
-      <c r="G12" s="34">
-        <f t="shared" ref="G12:G15" si="0">IFERROR((E12/86400)+DATE(1970,1,1),"&lt;== After")</f>
+      <c r="G12" s="30">
+        <f t="shared" ref="G12:G14" si="0">IFERROR((E12/86400)+DATE(1970,1,1),"&lt;== After")</f>
         <v>45207.368749999994</v>
       </c>
-      <c r="H12" s="13">
+      <c r="H12" s="11">
         <f>IFERROR($G$5*C12,"--")</f>
         <v>10</v>
       </c>
-      <c r="I12" s="13">
+      <c r="I12" s="11">
         <f>IFERROR($G$5*C12,"--")</f>
         <v>10</v>
       </c>
@@ -1051,10 +1051,10 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="7">
         <v>0.8</v>
       </c>
       <c r="D13" s="3">
@@ -1065,19 +1065,19 @@
         <f>+D13+(20*$C$2)-1</f>
         <v>1696756259.9999998</v>
       </c>
-      <c r="F13" s="34">
+      <c r="F13" s="30">
         <f t="shared" ref="F13:F15" si="1">IFERROR((D13/86400)+DATE(1970,1,1),_xlfn.CONCAT("Before ==&gt;"))</f>
         <v>45207.368761574071</v>
       </c>
-      <c r="G13" s="34">
+      <c r="G13" s="30">
         <f t="shared" si="0"/>
         <v>45207.382638888885</v>
       </c>
-      <c r="H13" s="13">
+      <c r="H13" s="11">
         <f>IFERROR($G$5*C13,"--")</f>
         <v>8</v>
       </c>
-      <c r="I13" s="13">
+      <c r="I13" s="11">
         <f>IFERROR($G$5*C13,"--")</f>
         <v>8</v>
       </c>
@@ -1086,10 +1086,10 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="7">
         <v>0.4</v>
       </c>
       <c r="D14" s="3">
@@ -1100,19 +1100,19 @@
         <f>+D14+(2*$C$2)-1</f>
         <v>1696756379.9999998</v>
       </c>
-      <c r="F14" s="34">
+      <c r="F14" s="30">
         <f t="shared" si="1"/>
         <v>45207.382650462961</v>
       </c>
-      <c r="G14" s="34">
+      <c r="G14" s="30">
         <f t="shared" si="0"/>
         <v>45207.384027777778</v>
       </c>
-      <c r="H14" s="13">
+      <c r="H14" s="11">
         <f>IFERROR($G$5*C14,"--")</f>
         <v>4</v>
       </c>
-      <c r="I14" s="13">
+      <c r="I14" s="11">
         <f>IFERROR($G$5*C14,"--")</f>
         <v>4</v>
       </c>
@@ -1121,32 +1121,32 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="9" t="s">
         <v>27</v>
       </c>
       <c r="D15" s="3">
         <f>E14+1</f>
         <v>1696756380.9999998</v>
       </c>
-      <c r="E15" s="27" t="s">
+      <c r="E15" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="F15" s="34">
+      <c r="F15" s="30">
         <f t="shared" si="1"/>
         <v>45207.384039351848</v>
       </c>
-      <c r="G15" s="34" t="str">
+      <c r="G15" s="30" t="str">
         <f>IFERROR((E15/86400)+DATE(1970,1,1),"&lt;== After")</f>
         <v>&lt;== After</v>
       </c>
-      <c r="H15" s="13" t="str">
+      <c r="H15" s="11" t="str">
         <f>IFERROR($G$5*C15,"--")</f>
         <v>--</v>
       </c>
-      <c r="I15" s="13" t="str">
+      <c r="I15" s="11" t="str">
         <f>IFERROR($G$5*C15,"--")</f>
         <v>--</v>
       </c>
@@ -1160,76 +1160,76 @@
       </c>
     </row>
     <row r="19" spans="2:10" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D19" s="25" t="s">
+      <c r="D19" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="26"/>
-      <c r="F19" s="5" t="s">
+      <c r="E19" s="32"/>
+      <c r="F19" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5" t="s">
+      <c r="G19" s="33"/>
+      <c r="H19" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="I19" s="5"/>
+      <c r="I19" s="33"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B20" s="10"/>
-      <c r="C20" s="7" t="s">
+      <c r="B20" s="34"/>
+      <c r="C20" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D20" s="24" t="s">
+      <c r="D20" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="E20" s="23" t="s">
+      <c r="E20" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G20" s="6" t="s">
+      <c r="G20" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="H20" s="6" t="s">
+      <c r="H20" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I20" s="6" t="s">
+      <c r="I20" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="8">
+      <c r="C21" s="7">
         <v>0</v>
       </c>
-      <c r="D21" s="27" t="s">
+      <c r="D21" s="23" t="s">
         <v>26</v>
       </c>
       <c r="E21" s="3">
         <f>$D$6+(2*($C$2))-1</f>
         <v>1696756618.9999998</v>
       </c>
-      <c r="F21" s="34" t="str">
+      <c r="F21" s="30" t="str">
         <f t="shared" ref="F21:F25" si="2">IFERROR((D21/86400)+DATE(1970,1,1),_xlfn.CONCAT("Before ==&gt;"))</f>
         <v>Before ==&gt;</v>
       </c>
-      <c r="G21" s="34">
+      <c r="G21" s="30">
         <f t="shared" ref="G21:G25" si="3">IFERROR((E21/86400)+DATE(1970,1,1),"&lt;== After")</f>
         <v>45207.386793981481</v>
       </c>
-      <c r="H21" s="13">
+      <c r="H21" s="11">
         <f>+$G$5*C21</f>
         <v>0</v>
       </c>
-      <c r="I21" s="13">
+      <c r="I21" s="11">
         <f>$G$5-H21</f>
         <v>10</v>
       </c>
@@ -1238,10 +1238,10 @@
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="8">
+      <c r="C22" s="7">
         <v>0.1</v>
       </c>
       <c r="D22" s="3">
@@ -1252,19 +1252,19 @@
         <f>+D22+(10*$C$2)-1</f>
         <v>1696757218.9999998</v>
       </c>
-      <c r="F22" s="34">
+      <c r="F22" s="30">
         <f t="shared" si="2"/>
         <v>45207.38680555555</v>
       </c>
-      <c r="G22" s="34">
+      <c r="G22" s="30">
         <f t="shared" si="3"/>
         <v>45207.393738425919</v>
       </c>
-      <c r="H22" s="13">
+      <c r="H22" s="11">
         <f>+$G$5*C22</f>
         <v>1</v>
       </c>
-      <c r="I22" s="13">
+      <c r="I22" s="11">
         <f>$G$5-H22</f>
         <v>9</v>
       </c>
@@ -1273,10 +1273,10 @@
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="8">
+      <c r="C23" s="7">
         <v>0.4</v>
       </c>
       <c r="D23" s="3">
@@ -1287,19 +1287,19 @@
         <f>+D23+(10*$C$2)-1</f>
         <v>1696757818.9999998</v>
       </c>
-      <c r="F23" s="34">
+      <c r="F23" s="30">
         <f t="shared" si="2"/>
         <v>45207.393749999996</v>
       </c>
-      <c r="G23" s="34">
+      <c r="G23" s="30">
         <f t="shared" si="3"/>
         <v>45207.400682870371</v>
       </c>
-      <c r="H23" s="13">
+      <c r="H23" s="11">
         <f>+$G$5*C23</f>
         <v>4</v>
       </c>
-      <c r="I23" s="13">
+      <c r="I23" s="11">
         <f>$G$5-H23</f>
         <v>6</v>
       </c>
@@ -1308,32 +1308,32 @@
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C24" s="8">
+      <c r="C24" s="7">
         <v>1</v>
       </c>
       <c r="D24" s="3">
         <f>+E23+1</f>
         <v>1696757819.9999998</v>
       </c>
-      <c r="E24" s="27" t="s">
+      <c r="E24" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="F24" s="34">
+      <c r="F24" s="30">
         <f t="shared" si="2"/>
         <v>45207.400694444441</v>
       </c>
-      <c r="G24" s="34" t="str">
+      <c r="G24" s="30" t="str">
         <f t="shared" si="3"/>
         <v>&lt;== After</v>
       </c>
-      <c r="H24" s="13">
+      <c r="H24" s="11">
         <f>+$G$5*C24</f>
         <v>10</v>
       </c>
-      <c r="I24" s="13">
+      <c r="I24" s="11">
         <f>$G$5-H24</f>
         <v>0</v>
       </c>
@@ -1342,10 +1342,10 @@
       </c>
     </row>
     <row r="25" spans="2:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="8">
+      <c r="C25" s="7">
         <v>1</v>
       </c>
       <c r="D25" s="3">
@@ -1356,19 +1356,19 @@
         <f>$D$6-1</f>
         <v>1696756498.9999998</v>
       </c>
-      <c r="F25" s="34">
+      <c r="F25" s="30">
         <f t="shared" si="2"/>
         <v>45207.368749999994</v>
       </c>
-      <c r="G25" s="34">
+      <c r="G25" s="30">
         <f t="shared" si="3"/>
         <v>45207.385405092587</v>
       </c>
-      <c r="H25" s="13">
+      <c r="H25" s="11">
         <f>+$G$5*C25</f>
         <v>10</v>
       </c>
-      <c r="I25" s="13">
+      <c r="I25" s="11">
         <f>$G$5-H25</f>
         <v>0</v>
       </c>
@@ -1378,14 +1378,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B19:B20"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="F10:G10"/>
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="D19:E19"/>
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="H19:I19"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B19:B20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1420,34 +1420,34 @@
       <c r="C1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="15">
+      <c r="D1" s="13">
         <v>60</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="13" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C2" s="16">
+      <c r="C2" s="14">
         <f>+D1</f>
         <v>60</v>
       </c>
-      <c r="D2" s="17">
+      <c r="D2" s="15">
         <f>+D1*60</f>
         <v>3600</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="15" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="10" t="s">
         <v>28</v>
       </c>
       <c r="C3" s="2"/>
@@ -1455,31 +1455,31 @@
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="29" t="s">
+      <c r="E4" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="30" t="s">
+      <c r="G4" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="21" t="s">
+      <c r="H4" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="I4" s="21" t="s">
+      <c r="I4" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="J4" s="21" t="s">
+      <c r="J4" s="19" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1487,24 +1487,24 @@
       <c r="B5" s="3">
         <v>112</v>
       </c>
-      <c r="C5" s="32" t="str">
+      <c r="C5" s="28" t="str">
         <f>_xlfn.CONCAT("D",B5)</f>
         <v>D112</v>
       </c>
-      <c r="D5" s="33">
+      <c r="D5" s="29">
         <v>45207.385416666664</v>
       </c>
       <c r="E5" s="2">
         <v>2</v>
       </c>
-      <c r="F5" s="33">
+      <c r="F5" s="29">
         <f>D5+E5/24</f>
         <v>45207.46875</v>
       </c>
-      <c r="G5" s="20">
+      <c r="G5" s="18">
         <v>10</v>
       </c>
-      <c r="H5" s="28" t="s">
+      <c r="H5" s="24" t="s">
         <v>13</v>
       </c>
       <c r="I5" s="2" t="s">
@@ -1515,25 +1515,25 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="31" t="str">
+      <c r="B6" s="27" t="str">
         <f>_xlfn.CONCAT(B5,",",C5,",",D6,",",F6,",",I5,",",J5)</f>
         <v>112,D112,1696756500,1696763700,DEL,CCU</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="17">
         <f>(D5-25569)*86400</f>
         <v>1696756499.9999998</v>
       </c>
-      <c r="F6" s="19">
+      <c r="F6" s="17">
         <f>(F5-25569)*86400</f>
         <v>1696763700</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="12">
         <f>G5*1000000000000000000</f>
         <v>1E+19</v>
       </c>
@@ -1542,14 +1542,14 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="34">
+      <c r="D7" s="30">
         <f>(D6/86400)+DATE(1970,1,1)</f>
         <v>45207.385416666664</v>
       </c>
-      <c r="F7" s="34">
+      <c r="F7" s="30">
         <f>(F6/86400)+DATE(1970,1,1)</f>
         <v>45207.46875</v>
       </c>
@@ -1560,76 +1560,76 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="D10" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="26"/>
-      <c r="F10" s="5" t="s">
+      <c r="E10" s="32"/>
+      <c r="F10" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5" t="s">
+      <c r="G10" s="33"/>
+      <c r="H10" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="I10" s="5"/>
+      <c r="I10" s="33"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B11" s="10"/>
-      <c r="C11" s="7" t="s">
+      <c r="B11" s="34"/>
+      <c r="C11" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="24" t="s">
+      <c r="D11" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="23" t="s">
+      <c r="E11" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="I11" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="7">
         <v>1</v>
       </c>
-      <c r="D12" s="27" t="s">
+      <c r="D12" s="23" t="s">
         <v>26</v>
       </c>
       <c r="E12" s="3">
         <f>$D$6-(24*($C$2))</f>
         <v>1696755059.9999998</v>
       </c>
-      <c r="F12" s="34" t="str">
+      <c r="F12" s="30" t="str">
         <f>IFERROR((D12/86400)+DATE(1970,1,1),_xlfn.CONCAT("Before ==&gt;"))</f>
         <v>Before ==&gt;</v>
       </c>
-      <c r="G12" s="34">
-        <f t="shared" ref="G12:G15" si="0">IFERROR((E12/86400)+DATE(1970,1,1),"&lt;== After")</f>
+      <c r="G12" s="30">
+        <f t="shared" ref="G12:G14" si="0">IFERROR((E12/86400)+DATE(1970,1,1),"&lt;== After")</f>
         <v>45207.368749999994</v>
       </c>
-      <c r="H12" s="13">
+      <c r="H12" s="11">
         <f>IFERROR($G$5*C12,"--")</f>
         <v>10</v>
       </c>
-      <c r="I12" s="13">
+      <c r="I12" s="11">
         <f>IFERROR($G$5*C12,"--")</f>
         <v>10</v>
       </c>
@@ -1638,10 +1638,10 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="7">
         <v>0.8</v>
       </c>
       <c r="D13" s="3">
@@ -1652,19 +1652,19 @@
         <f>+D13+(20*$C$2)-1</f>
         <v>1696756259.9999998</v>
       </c>
-      <c r="F13" s="34">
+      <c r="F13" s="30">
         <f t="shared" ref="F13:F15" si="1">IFERROR((D13/86400)+DATE(1970,1,1),_xlfn.CONCAT("Before ==&gt;"))</f>
         <v>45207.368761574071</v>
       </c>
-      <c r="G13" s="34">
+      <c r="G13" s="30">
         <f t="shared" si="0"/>
         <v>45207.382638888885</v>
       </c>
-      <c r="H13" s="13">
+      <c r="H13" s="11">
         <f>IFERROR($G$5*C13,"--")</f>
         <v>8</v>
       </c>
-      <c r="I13" s="13">
+      <c r="I13" s="11">
         <f>IFERROR($G$5*C13,"--")</f>
         <v>8</v>
       </c>
@@ -1673,10 +1673,10 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="7">
         <v>0.4</v>
       </c>
       <c r="D14" s="3">
@@ -1687,19 +1687,19 @@
         <f>+D14+(2*$C$2)-1</f>
         <v>1696756379.9999998</v>
       </c>
-      <c r="F14" s="34">
+      <c r="F14" s="30">
         <f t="shared" si="1"/>
         <v>45207.382650462961</v>
       </c>
-      <c r="G14" s="34">
+      <c r="G14" s="30">
         <f t="shared" si="0"/>
         <v>45207.384027777778</v>
       </c>
-      <c r="H14" s="13">
+      <c r="H14" s="11">
         <f>IFERROR($G$5*C14,"--")</f>
         <v>4</v>
       </c>
-      <c r="I14" s="13">
+      <c r="I14" s="11">
         <f>IFERROR($G$5*C14,"--")</f>
         <v>4</v>
       </c>
@@ -1708,32 +1708,32 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="9" t="s">
         <v>27</v>
       </c>
       <c r="D15" s="3">
         <f>E14+1</f>
         <v>1696756380.9999998</v>
       </c>
-      <c r="E15" s="27" t="s">
+      <c r="E15" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="F15" s="34">
+      <c r="F15" s="30">
         <f t="shared" si="1"/>
         <v>45207.384039351848</v>
       </c>
-      <c r="G15" s="34" t="str">
+      <c r="G15" s="30" t="str">
         <f>IFERROR((E15/86400)+DATE(1970,1,1),"&lt;== After")</f>
         <v>&lt;== After</v>
       </c>
-      <c r="H15" s="13" t="str">
+      <c r="H15" s="11" t="str">
         <f>IFERROR($G$5*C15,"--")</f>
         <v>--</v>
       </c>
-      <c r="I15" s="13" t="str">
+      <c r="I15" s="11" t="str">
         <f>IFERROR($G$5*C15,"--")</f>
         <v>--</v>
       </c>
@@ -1747,76 +1747,76 @@
       </c>
     </row>
     <row r="19" spans="2:10" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D19" s="25" t="s">
+      <c r="D19" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="26"/>
-      <c r="F19" s="5" t="s">
+      <c r="E19" s="32"/>
+      <c r="F19" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5" t="s">
+      <c r="G19" s="33"/>
+      <c r="H19" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="I19" s="5"/>
+      <c r="I19" s="33"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B20" s="10"/>
-      <c r="C20" s="7" t="s">
+      <c r="B20" s="34"/>
+      <c r="C20" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D20" s="24" t="s">
+      <c r="D20" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="E20" s="23" t="s">
+      <c r="E20" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G20" s="6" t="s">
+      <c r="G20" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="H20" s="6" t="s">
+      <c r="H20" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I20" s="6" t="s">
+      <c r="I20" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="8">
+      <c r="C21" s="7">
         <v>0</v>
       </c>
-      <c r="D21" s="27" t="s">
+      <c r="D21" s="23" t="s">
         <v>26</v>
       </c>
       <c r="E21" s="3">
         <f>$D$6+(2*($C$2))-1</f>
         <v>1696756618.9999998</v>
       </c>
-      <c r="F21" s="34" t="str">
+      <c r="F21" s="30" t="str">
         <f t="shared" ref="F21:F25" si="2">IFERROR((D21/86400)+DATE(1970,1,1),_xlfn.CONCAT("Before ==&gt;"))</f>
         <v>Before ==&gt;</v>
       </c>
-      <c r="G21" s="34">
+      <c r="G21" s="30">
         <f t="shared" ref="G21:G25" si="3">IFERROR((E21/86400)+DATE(1970,1,1),"&lt;== After")</f>
         <v>45207.386793981481</v>
       </c>
-      <c r="H21" s="13">
+      <c r="H21" s="11">
         <f>+$G$5*C21</f>
         <v>0</v>
       </c>
-      <c r="I21" s="13">
+      <c r="I21" s="11">
         <f>$G$5-H21</f>
         <v>10</v>
       </c>
@@ -1825,10 +1825,10 @@
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="8">
+      <c r="C22" s="7">
         <v>0.1</v>
       </c>
       <c r="D22" s="3">
@@ -1839,19 +1839,19 @@
         <f>+D22+(10*$C$2)-1</f>
         <v>1696757218.9999998</v>
       </c>
-      <c r="F22" s="34">
+      <c r="F22" s="30">
         <f t="shared" si="2"/>
         <v>45207.38680555555</v>
       </c>
-      <c r="G22" s="34">
+      <c r="G22" s="30">
         <f t="shared" si="3"/>
         <v>45207.393738425919</v>
       </c>
-      <c r="H22" s="13">
+      <c r="H22" s="11">
         <f>+$G$5*C22</f>
         <v>1</v>
       </c>
-      <c r="I22" s="13">
+      <c r="I22" s="11">
         <f>$G$5-H22</f>
         <v>9</v>
       </c>
@@ -1860,10 +1860,10 @@
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="8">
+      <c r="C23" s="7">
         <v>0.4</v>
       </c>
       <c r="D23" s="3">
@@ -1874,19 +1874,19 @@
         <f>+D23+(10*$C$2)-1</f>
         <v>1696757818.9999998</v>
       </c>
-      <c r="F23" s="34">
+      <c r="F23" s="30">
         <f t="shared" si="2"/>
         <v>45207.393749999996</v>
       </c>
-      <c r="G23" s="34">
+      <c r="G23" s="30">
         <f t="shared" si="3"/>
         <v>45207.400682870371</v>
       </c>
-      <c r="H23" s="13">
+      <c r="H23" s="11">
         <f>+$G$5*C23</f>
         <v>4</v>
       </c>
-      <c r="I23" s="13">
+      <c r="I23" s="11">
         <f>$G$5-H23</f>
         <v>6</v>
       </c>
@@ -1895,32 +1895,32 @@
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C24" s="8">
+      <c r="C24" s="7">
         <v>1</v>
       </c>
       <c r="D24" s="3">
         <f>+E23+1</f>
         <v>1696757819.9999998</v>
       </c>
-      <c r="E24" s="27" t="s">
+      <c r="E24" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="F24" s="34">
+      <c r="F24" s="30">
         <f t="shared" si="2"/>
         <v>45207.400694444441</v>
       </c>
-      <c r="G24" s="34" t="str">
+      <c r="G24" s="30" t="str">
         <f t="shared" si="3"/>
         <v>&lt;== After</v>
       </c>
-      <c r="H24" s="13">
+      <c r="H24" s="11">
         <f>+$G$5*C24</f>
         <v>10</v>
       </c>
-      <c r="I24" s="13">
+      <c r="I24" s="11">
         <f>$G$5-H24</f>
         <v>0</v>
       </c>
@@ -1929,10 +1929,10 @@
       </c>
     </row>
     <row r="25" spans="2:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="8">
+      <c r="C25" s="7">
         <v>1</v>
       </c>
       <c r="D25" s="3">
@@ -1943,19 +1943,19 @@
         <f>$D$6-1</f>
         <v>1696756498.9999998</v>
       </c>
-      <c r="F25" s="34">
+      <c r="F25" s="30">
         <f t="shared" si="2"/>
         <v>45207.368749999994</v>
       </c>
-      <c r="G25" s="34">
+      <c r="G25" s="30">
         <f t="shared" si="3"/>
         <v>45207.385405092587</v>
       </c>
-      <c r="H25" s="13">
+      <c r="H25" s="11">
         <f>+$G$5*C25</f>
         <v>10</v>
       </c>
-      <c r="I25" s="13">
+      <c r="I25" s="11">
         <f>$G$5-H25</f>
         <v>0</v>
       </c>
@@ -2007,34 +2007,34 @@
       <c r="C1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="15">
+      <c r="D1" s="13">
         <v>60</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="13" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C2" s="16">
+      <c r="C2" s="14">
         <f>D1</f>
         <v>60</v>
       </c>
-      <c r="D2" s="17">
+      <c r="D2" s="15">
         <f>+D1*60</f>
         <v>3600</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="15" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="10" t="s">
         <v>28</v>
       </c>
       <c r="C3" s="2"/>
@@ -2042,31 +2042,31 @@
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="29" t="s">
+      <c r="E4" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="30" t="s">
+      <c r="G4" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="21" t="s">
+      <c r="H4" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="I4" s="21" t="s">
+      <c r="I4" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="J4" s="21" t="s">
+      <c r="J4" s="19" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2074,24 +2074,24 @@
       <c r="B5" s="3">
         <v>123</v>
       </c>
-      <c r="C5" s="32" t="str">
+      <c r="C5" s="28" t="str">
         <f>_xlfn.CONCAT("D",B5)</f>
         <v>D123</v>
       </c>
-      <c r="D5" s="33">
+      <c r="D5" s="29">
         <v>45207.385416666664</v>
       </c>
       <c r="E5" s="2">
         <v>2</v>
       </c>
-      <c r="F5" s="33">
+      <c r="F5" s="29">
         <f>D5+E5/24</f>
         <v>45207.46875</v>
       </c>
-      <c r="G5" s="20">
+      <c r="G5" s="18">
         <v>10</v>
       </c>
-      <c r="H5" s="28" t="s">
+      <c r="H5" s="24" t="s">
         <v>13</v>
       </c>
       <c r="I5" s="2" t="s">
@@ -2102,25 +2102,25 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="31" t="str">
+      <c r="B6" s="27" t="str">
         <f>_xlfn.CONCAT(B5,",",C5,",",D6,",",F6,",",I5,",",J5)</f>
         <v>123,D123,1696756500,1696763700,MAA,CCU</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="17">
         <f>(D5-25569)*86400</f>
         <v>1696756499.9999998</v>
       </c>
-      <c r="F6" s="19">
+      <c r="F6" s="17">
         <f>(F5-25569)*86400</f>
         <v>1696763700</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="12">
         <f>G5*1000000000000000000</f>
         <v>1E+19</v>
       </c>
@@ -2129,7 +2129,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="10" t="s">
         <v>30</v>
       </c>
       <c r="D7" s="4">
@@ -2147,76 +2147,76 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="D10" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="26"/>
-      <c r="F10" s="5" t="s">
+      <c r="E10" s="32"/>
+      <c r="F10" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5" t="s">
+      <c r="G10" s="33"/>
+      <c r="H10" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="I10" s="5"/>
+      <c r="I10" s="33"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B11" s="10"/>
-      <c r="C11" s="7" t="s">
+      <c r="B11" s="34"/>
+      <c r="C11" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="24" t="s">
+      <c r="D11" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="23" t="s">
+      <c r="E11" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="I11" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="7">
         <v>1</v>
       </c>
-      <c r="D12" s="27" t="s">
+      <c r="D12" s="23" t="s">
         <v>26</v>
       </c>
       <c r="E12" s="3">
         <f>$D$6-(24*($C$2))</f>
         <v>1696755059.9999998</v>
       </c>
-      <c r="F12" s="34" t="str">
+      <c r="F12" s="30" t="str">
         <f>IFERROR((D12/86400)+DATE(1970,1,1),_xlfn.CONCAT("Before ==&gt;"))</f>
         <v>Before ==&gt;</v>
       </c>
-      <c r="G12" s="34">
-        <f t="shared" ref="G12:G15" si="0">IFERROR((E12/86400)+DATE(1970,1,1),"&lt;== After")</f>
+      <c r="G12" s="30">
+        <f t="shared" ref="G12:G14" si="0">IFERROR((E12/86400)+DATE(1970,1,1),"&lt;== After")</f>
         <v>45207.368749999994</v>
       </c>
-      <c r="H12" s="13">
+      <c r="H12" s="11">
         <f>IFERROR($G$5*C12,"--")</f>
         <v>10</v>
       </c>
-      <c r="I12" s="13">
+      <c r="I12" s="11">
         <f>IFERROR($G$5*C12,"--")</f>
         <v>10</v>
       </c>
@@ -2225,10 +2225,10 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="7">
         <v>0.8</v>
       </c>
       <c r="D13" s="3">
@@ -2239,19 +2239,19 @@
         <f>+D13+(20*$C$2)-1</f>
         <v>1696756259.9999998</v>
       </c>
-      <c r="F13" s="34">
+      <c r="F13" s="30">
         <f t="shared" ref="F13:F15" si="1">IFERROR((D13/86400)+DATE(1970,1,1),_xlfn.CONCAT("Before ==&gt;"))</f>
         <v>45207.368761574071</v>
       </c>
-      <c r="G13" s="34">
+      <c r="G13" s="30">
         <f t="shared" si="0"/>
         <v>45207.382638888885</v>
       </c>
-      <c r="H13" s="13">
+      <c r="H13" s="11">
         <f>IFERROR($G$5*C13,"--")</f>
         <v>8</v>
       </c>
-      <c r="I13" s="13">
+      <c r="I13" s="11">
         <f>IFERROR($G$5*C13,"--")</f>
         <v>8</v>
       </c>
@@ -2260,10 +2260,10 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="7">
         <v>0.4</v>
       </c>
       <c r="D14" s="3">
@@ -2274,19 +2274,19 @@
         <f>+D14+(2*$C$2)-1</f>
         <v>1696756379.9999998</v>
       </c>
-      <c r="F14" s="34">
+      <c r="F14" s="30">
         <f t="shared" si="1"/>
         <v>45207.382650462961</v>
       </c>
-      <c r="G14" s="34">
+      <c r="G14" s="30">
         <f t="shared" si="0"/>
         <v>45207.384027777778</v>
       </c>
-      <c r="H14" s="13">
+      <c r="H14" s="11">
         <f>IFERROR($G$5*C14,"--")</f>
         <v>4</v>
       </c>
-      <c r="I14" s="13">
+      <c r="I14" s="11">
         <f>IFERROR($G$5*C14,"--")</f>
         <v>4</v>
       </c>
@@ -2295,32 +2295,32 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="9" t="s">
         <v>27</v>
       </c>
       <c r="D15" s="3">
         <f>E14+1</f>
         <v>1696756380.9999998</v>
       </c>
-      <c r="E15" s="27" t="s">
+      <c r="E15" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="F15" s="34">
+      <c r="F15" s="30">
         <f t="shared" si="1"/>
         <v>45207.384039351848</v>
       </c>
-      <c r="G15" s="34" t="str">
+      <c r="G15" s="30" t="str">
         <f>IFERROR((E15/86400)+DATE(1970,1,1),"&lt;== After")</f>
         <v>&lt;== After</v>
       </c>
-      <c r="H15" s="13" t="str">
+      <c r="H15" s="11" t="str">
         <f>IFERROR($G$5*C15,"--")</f>
         <v>--</v>
       </c>
-      <c r="I15" s="13" t="str">
+      <c r="I15" s="11" t="str">
         <f>IFERROR($G$5*C15,"--")</f>
         <v>--</v>
       </c>
@@ -2334,76 +2334,76 @@
       </c>
     </row>
     <row r="19" spans="2:10" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D19" s="25" t="s">
+      <c r="D19" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="26"/>
-      <c r="F19" s="5" t="s">
+      <c r="E19" s="32"/>
+      <c r="F19" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5" t="s">
+      <c r="G19" s="33"/>
+      <c r="H19" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="I19" s="5"/>
+      <c r="I19" s="33"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B20" s="10"/>
-      <c r="C20" s="7" t="s">
+      <c r="B20" s="34"/>
+      <c r="C20" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D20" s="24" t="s">
+      <c r="D20" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="E20" s="23" t="s">
+      <c r="E20" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G20" s="6" t="s">
+      <c r="G20" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="H20" s="6" t="s">
+      <c r="H20" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I20" s="6" t="s">
+      <c r="I20" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="8">
+      <c r="C21" s="7">
         <v>0</v>
       </c>
-      <c r="D21" s="27" t="s">
+      <c r="D21" s="23" t="s">
         <v>26</v>
       </c>
       <c r="E21" s="3">
         <f>$D$6+(2*($C$2))-1</f>
         <v>1696756618.9999998</v>
       </c>
-      <c r="F21" s="34" t="str">
+      <c r="F21" s="30" t="str">
         <f t="shared" ref="F21:F25" si="2">IFERROR((D21/86400)+DATE(1970,1,1),_xlfn.CONCAT("Before ==&gt;"))</f>
         <v>Before ==&gt;</v>
       </c>
-      <c r="G21" s="34">
+      <c r="G21" s="30">
         <f t="shared" ref="G21:G25" si="3">IFERROR((E21/86400)+DATE(1970,1,1),"&lt;== After")</f>
         <v>45207.386793981481</v>
       </c>
-      <c r="H21" s="13">
+      <c r="H21" s="11">
         <f>+$G$5*C21</f>
         <v>0</v>
       </c>
-      <c r="I21" s="13">
+      <c r="I21" s="11">
         <f>$G$5-H21</f>
         <v>10</v>
       </c>
@@ -2412,10 +2412,10 @@
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="8">
+      <c r="C22" s="7">
         <v>0.1</v>
       </c>
       <c r="D22" s="3">
@@ -2426,19 +2426,19 @@
         <f>+D22+(10*$C$2)-1</f>
         <v>1696757218.9999998</v>
       </c>
-      <c r="F22" s="34">
+      <c r="F22" s="30">
         <f t="shared" si="2"/>
         <v>45207.38680555555</v>
       </c>
-      <c r="G22" s="34">
+      <c r="G22" s="30">
         <f t="shared" si="3"/>
         <v>45207.393738425919</v>
       </c>
-      <c r="H22" s="13">
+      <c r="H22" s="11">
         <f>+$G$5*C22</f>
         <v>1</v>
       </c>
-      <c r="I22" s="13">
+      <c r="I22" s="11">
         <f>$G$5-H22</f>
         <v>9</v>
       </c>
@@ -2447,10 +2447,10 @@
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="8">
+      <c r="C23" s="7">
         <v>0.4</v>
       </c>
       <c r="D23" s="3">
@@ -2461,19 +2461,19 @@
         <f>+D23+(10*$C$2)-1</f>
         <v>1696757818.9999998</v>
       </c>
-      <c r="F23" s="34">
+      <c r="F23" s="30">
         <f t="shared" si="2"/>
         <v>45207.393749999996</v>
       </c>
-      <c r="G23" s="34">
+      <c r="G23" s="30">
         <f t="shared" si="3"/>
         <v>45207.400682870371</v>
       </c>
-      <c r="H23" s="13">
+      <c r="H23" s="11">
         <f>+$G$5*C23</f>
         <v>4</v>
       </c>
-      <c r="I23" s="13">
+      <c r="I23" s="11">
         <f>$G$5-H23</f>
         <v>6</v>
       </c>
@@ -2482,32 +2482,32 @@
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C24" s="8">
+      <c r="C24" s="7">
         <v>1</v>
       </c>
       <c r="D24" s="3">
         <f>+E23+1</f>
         <v>1696757819.9999998</v>
       </c>
-      <c r="E24" s="27" t="s">
+      <c r="E24" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="F24" s="34">
+      <c r="F24" s="30">
         <f t="shared" si="2"/>
         <v>45207.400694444441</v>
       </c>
-      <c r="G24" s="34" t="str">
+      <c r="G24" s="30" t="str">
         <f t="shared" si="3"/>
         <v>&lt;== After</v>
       </c>
-      <c r="H24" s="13">
+      <c r="H24" s="11">
         <f>+$G$5*C24</f>
         <v>10</v>
       </c>
-      <c r="I24" s="13">
+      <c r="I24" s="11">
         <f>$G$5-H24</f>
         <v>0</v>
       </c>
@@ -2516,10 +2516,10 @@
       </c>
     </row>
     <row r="25" spans="2:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="8">
+      <c r="C25" s="7">
         <v>1</v>
       </c>
       <c r="D25" s="3">
@@ -2530,19 +2530,19 @@
         <f>$D$6-1</f>
         <v>1696756498.9999998</v>
       </c>
-      <c r="F25" s="34">
+      <c r="F25" s="30">
         <f t="shared" si="2"/>
         <v>45207.368749999994</v>
       </c>
-      <c r="G25" s="34">
+      <c r="G25" s="30">
         <f t="shared" si="3"/>
         <v>45207.385405092587</v>
       </c>
-      <c r="H25" s="13">
+      <c r="H25" s="11">
         <f>+$G$5*C25</f>
         <v>10</v>
       </c>
-      <c r="I25" s="13">
+      <c r="I25" s="11">
         <f>$G$5-H25</f>
         <v>0</v>
       </c>
@@ -2593,34 +2593,34 @@
       <c r="C1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="15">
+      <c r="D1" s="13">
         <v>60</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="13" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C2" s="16">
+      <c r="C2" s="14">
         <f>D1</f>
         <v>60</v>
       </c>
-      <c r="D2" s="17">
+      <c r="D2" s="15">
         <f>+D1*60</f>
         <v>3600</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="15" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="10" t="s">
         <v>28</v>
       </c>
       <c r="C3" s="2"/>
@@ -2628,31 +2628,31 @@
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="29" t="s">
+      <c r="E4" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="30" t="s">
+      <c r="G4" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="21" t="s">
+      <c r="H4" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="I4" s="21" t="s">
+      <c r="I4" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="J4" s="21" t="s">
+      <c r="J4" s="19" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2660,24 +2660,24 @@
       <c r="B5" s="3">
         <v>201</v>
       </c>
-      <c r="C5" s="32" t="str">
+      <c r="C5" s="28" t="str">
         <f>_xlfn.CONCAT("I",B5)</f>
         <v>I201</v>
       </c>
-      <c r="D5" s="33">
+      <c r="D5" s="29">
         <v>45207.385416666664</v>
       </c>
       <c r="E5" s="2">
         <v>24</v>
       </c>
-      <c r="F5" s="33">
+      <c r="F5" s="29">
         <f>D5+E5/24</f>
         <v>45208.385416666664</v>
       </c>
-      <c r="G5" s="20">
+      <c r="G5" s="18">
         <v>25</v>
       </c>
-      <c r="H5" s="28" t="s">
+      <c r="H5" s="24" t="s">
         <v>13</v>
       </c>
       <c r="I5" s="2" t="s">
@@ -2688,25 +2688,25 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="31" t="str">
+      <c r="B6" s="27" t="str">
         <f>_xlfn.CONCAT(B5,",",C5,",",D6,",",F6,",",I5,",",J5)</f>
         <v>201,I201,1696756500,1696842900,BOM,NYC</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="17">
         <f>(D5-25569)*86400</f>
         <v>1696756499.9999998</v>
       </c>
-      <c r="F6" s="19">
+      <c r="F6" s="17">
         <f>(F5-25569)*86400</f>
         <v>1696842899.9999998</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="12">
         <f>G5*1000000000000000000</f>
         <v>2.5E+19</v>
       </c>
@@ -2715,7 +2715,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="10" t="s">
         <v>30</v>
       </c>
       <c r="D7" s="4">
@@ -2733,76 +2733,76 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="D10" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="26"/>
-      <c r="F10" s="5" t="s">
+      <c r="E10" s="32"/>
+      <c r="F10" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5" t="s">
+      <c r="G10" s="33"/>
+      <c r="H10" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="I10" s="5"/>
+      <c r="I10" s="33"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B11" s="10"/>
-      <c r="C11" s="7" t="s">
+      <c r="B11" s="34"/>
+      <c r="C11" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="24" t="s">
+      <c r="D11" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="23" t="s">
+      <c r="E11" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="I11" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="7">
         <v>1</v>
       </c>
-      <c r="D12" s="27" t="s">
+      <c r="D12" s="23" t="s">
         <v>26</v>
       </c>
       <c r="E12" s="3">
         <f>$D$6-(24*($C$2))</f>
         <v>1696755059.9999998</v>
       </c>
-      <c r="F12" s="34" t="str">
+      <c r="F12" s="30" t="str">
         <f>IFERROR((D12/86400)+DATE(1970,1,1),_xlfn.CONCAT("Before ==&gt;"))</f>
         <v>Before ==&gt;</v>
       </c>
-      <c r="G12" s="34">
-        <f t="shared" ref="G12:G15" si="0">IFERROR((E12/86400)+DATE(1970,1,1),"&lt;== After")</f>
+      <c r="G12" s="30">
+        <f t="shared" ref="G12:G14" si="0">IFERROR((E12/86400)+DATE(1970,1,1),"&lt;== After")</f>
         <v>45207.368749999994</v>
       </c>
-      <c r="H12" s="13">
+      <c r="H12" s="11">
         <f>IFERROR($G$5*C12,"--")</f>
         <v>25</v>
       </c>
-      <c r="I12" s="13">
+      <c r="I12" s="11">
         <f>IFERROR($G$5*C12,"--")</f>
         <v>25</v>
       </c>
@@ -2811,10 +2811,10 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="7">
         <v>0.8</v>
       </c>
       <c r="D13" s="3">
@@ -2825,19 +2825,19 @@
         <f>+D13+(20*$C$2)-1</f>
         <v>1696756259.9999998</v>
       </c>
-      <c r="F13" s="34">
+      <c r="F13" s="30">
         <f t="shared" ref="F13:F15" si="1">IFERROR((D13/86400)+DATE(1970,1,1),_xlfn.CONCAT("Before ==&gt;"))</f>
         <v>45207.368761574071</v>
       </c>
-      <c r="G13" s="34">
+      <c r="G13" s="30">
         <f t="shared" si="0"/>
         <v>45207.382638888885</v>
       </c>
-      <c r="H13" s="13">
+      <c r="H13" s="11">
         <f>IFERROR($G$5*C13,"--")</f>
         <v>20</v>
       </c>
-      <c r="I13" s="13">
+      <c r="I13" s="11">
         <f>IFERROR($G$5*C13,"--")</f>
         <v>20</v>
       </c>
@@ -2846,10 +2846,10 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="7">
         <v>0.4</v>
       </c>
       <c r="D14" s="3">
@@ -2860,19 +2860,19 @@
         <f>+D14+(2*$C$2)-1</f>
         <v>1696756379.9999998</v>
       </c>
-      <c r="F14" s="34">
+      <c r="F14" s="30">
         <f t="shared" si="1"/>
         <v>45207.382650462961</v>
       </c>
-      <c r="G14" s="34">
+      <c r="G14" s="30">
         <f t="shared" si="0"/>
         <v>45207.384027777778</v>
       </c>
-      <c r="H14" s="13">
+      <c r="H14" s="11">
         <f>IFERROR($G$5*C14,"--")</f>
         <v>10</v>
       </c>
-      <c r="I14" s="13">
+      <c r="I14" s="11">
         <f>IFERROR($G$5*C14,"--")</f>
         <v>10</v>
       </c>
@@ -2881,32 +2881,32 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="9" t="s">
         <v>27</v>
       </c>
       <c r="D15" s="3">
         <f>E14+1</f>
         <v>1696756380.9999998</v>
       </c>
-      <c r="E15" s="27" t="s">
+      <c r="E15" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="F15" s="34">
+      <c r="F15" s="30">
         <f t="shared" si="1"/>
         <v>45207.384039351848</v>
       </c>
-      <c r="G15" s="34" t="str">
+      <c r="G15" s="30" t="str">
         <f>IFERROR((E15/86400)+DATE(1970,1,1),"&lt;== After")</f>
         <v>&lt;== After</v>
       </c>
-      <c r="H15" s="13" t="str">
+      <c r="H15" s="11" t="str">
         <f>IFERROR($G$5*C15,"--")</f>
         <v>--</v>
       </c>
-      <c r="I15" s="13" t="str">
+      <c r="I15" s="11" t="str">
         <f>IFERROR($G$5*C15,"--")</f>
         <v>--</v>
       </c>
@@ -2920,76 +2920,76 @@
       </c>
     </row>
     <row r="19" spans="2:10" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D19" s="25" t="s">
+      <c r="D19" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="26"/>
-      <c r="F19" s="5" t="s">
+      <c r="E19" s="32"/>
+      <c r="F19" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5" t="s">
+      <c r="G19" s="33"/>
+      <c r="H19" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="I19" s="5"/>
+      <c r="I19" s="33"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B20" s="10"/>
-      <c r="C20" s="7" t="s">
+      <c r="B20" s="34"/>
+      <c r="C20" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D20" s="24" t="s">
+      <c r="D20" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="E20" s="23" t="s">
+      <c r="E20" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G20" s="6" t="s">
+      <c r="G20" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="H20" s="6" t="s">
+      <c r="H20" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I20" s="6" t="s">
+      <c r="I20" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="8">
+      <c r="C21" s="7">
         <v>0</v>
       </c>
-      <c r="D21" s="27" t="s">
+      <c r="D21" s="23" t="s">
         <v>26</v>
       </c>
       <c r="E21" s="3">
         <f>$D$6+(2*($C$2))-1</f>
         <v>1696756618.9999998</v>
       </c>
-      <c r="F21" s="34" t="str">
+      <c r="F21" s="30" t="str">
         <f t="shared" ref="F21:F25" si="2">IFERROR((D21/86400)+DATE(1970,1,1),_xlfn.CONCAT("Before ==&gt;"))</f>
         <v>Before ==&gt;</v>
       </c>
-      <c r="G21" s="34">
+      <c r="G21" s="30">
         <f t="shared" ref="G21:G25" si="3">IFERROR((E21/86400)+DATE(1970,1,1),"&lt;== After")</f>
         <v>45207.386793981481</v>
       </c>
-      <c r="H21" s="13">
+      <c r="H21" s="11">
         <f>+$G$5*C21</f>
         <v>0</v>
       </c>
-      <c r="I21" s="13">
+      <c r="I21" s="11">
         <f>$G$5-H21</f>
         <v>25</v>
       </c>
@@ -2998,10 +2998,10 @@
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="8">
+      <c r="C22" s="7">
         <v>0.1</v>
       </c>
       <c r="D22" s="3">
@@ -3012,19 +3012,19 @@
         <f>+D22+(10*$C$2)-1</f>
         <v>1696757218.9999998</v>
       </c>
-      <c r="F22" s="34">
+      <c r="F22" s="30">
         <f t="shared" si="2"/>
         <v>45207.38680555555</v>
       </c>
-      <c r="G22" s="34">
+      <c r="G22" s="30">
         <f t="shared" si="3"/>
         <v>45207.393738425919</v>
       </c>
-      <c r="H22" s="13">
+      <c r="H22" s="11">
         <f>+$G$5*C22</f>
         <v>2.5</v>
       </c>
-      <c r="I22" s="13">
+      <c r="I22" s="11">
         <f>$G$5-H22</f>
         <v>22.5</v>
       </c>
@@ -3033,10 +3033,10 @@
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="8">
+      <c r="C23" s="7">
         <v>0.4</v>
       </c>
       <c r="D23" s="3">
@@ -3047,19 +3047,19 @@
         <f>+D23+(10*$C$2)-1</f>
         <v>1696757818.9999998</v>
       </c>
-      <c r="F23" s="34">
+      <c r="F23" s="30">
         <f t="shared" si="2"/>
         <v>45207.393749999996</v>
       </c>
-      <c r="G23" s="34">
+      <c r="G23" s="30">
         <f t="shared" si="3"/>
         <v>45207.400682870371</v>
       </c>
-      <c r="H23" s="13">
+      <c r="H23" s="11">
         <f>+$G$5*C23</f>
         <v>10</v>
       </c>
-      <c r="I23" s="13">
+      <c r="I23" s="11">
         <f>$G$5-H23</f>
         <v>15</v>
       </c>
@@ -3068,32 +3068,32 @@
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C24" s="8">
+      <c r="C24" s="7">
         <v>1</v>
       </c>
       <c r="D24" s="3">
         <f>+E23+1</f>
         <v>1696757819.9999998</v>
       </c>
-      <c r="E24" s="27" t="s">
+      <c r="E24" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="F24" s="34">
+      <c r="F24" s="30">
         <f t="shared" si="2"/>
         <v>45207.400694444441</v>
       </c>
-      <c r="G24" s="34" t="str">
+      <c r="G24" s="30" t="str">
         <f t="shared" si="3"/>
         <v>&lt;== After</v>
       </c>
-      <c r="H24" s="13">
+      <c r="H24" s="11">
         <f>+$G$5*C24</f>
         <v>25</v>
       </c>
-      <c r="I24" s="13">
+      <c r="I24" s="11">
         <f>$G$5-H24</f>
         <v>0</v>
       </c>
@@ -3102,10 +3102,10 @@
       </c>
     </row>
     <row r="25" spans="2:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="8">
+      <c r="C25" s="7">
         <v>1</v>
       </c>
       <c r="D25" s="3">
@@ -3116,19 +3116,19 @@
         <f>$D$6-1</f>
         <v>1696756498.9999998</v>
       </c>
-      <c r="F25" s="34">
+      <c r="F25" s="30">
         <f t="shared" si="2"/>
         <v>45207.368749999994</v>
       </c>
-      <c r="G25" s="34">
+      <c r="G25" s="30">
         <f t="shared" si="3"/>
         <v>45207.385405092587</v>
       </c>
-      <c r="H25" s="13">
+      <c r="H25" s="11">
         <f>+$G$5*C25</f>
         <v>25</v>
       </c>
-      <c r="I25" s="13">
+      <c r="I25" s="11">
         <f>$G$5-H25</f>
         <v>0</v>
       </c>
@@ -3179,34 +3179,34 @@
       <c r="C1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="15">
+      <c r="D1" s="13">
         <v>60</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="13" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C2" s="16">
+      <c r="C2" s="14">
         <f>D1</f>
         <v>60</v>
       </c>
-      <c r="D2" s="17">
+      <c r="D2" s="15">
         <f>+D1*60</f>
         <v>3600</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="15" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="10" t="s">
         <v>28</v>
       </c>
       <c r="C3" s="2"/>
@@ -3214,31 +3214,31 @@
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="29" t="s">
+      <c r="E4" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="30" t="s">
+      <c r="G4" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="21" t="s">
+      <c r="H4" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="I4" s="21" t="s">
+      <c r="I4" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="J4" s="21" t="s">
+      <c r="J4" s="19" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3246,24 +3246,24 @@
       <c r="B5" s="3">
         <v>212</v>
       </c>
-      <c r="C5" s="32" t="str">
+      <c r="C5" s="28" t="str">
         <f>_xlfn.CONCAT("I",B5)</f>
         <v>I212</v>
       </c>
-      <c r="D5" s="33">
+      <c r="D5" s="29">
         <v>45207.385416666664</v>
       </c>
       <c r="E5" s="2">
         <v>24</v>
       </c>
-      <c r="F5" s="33">
+      <c r="F5" s="29">
         <f>D5+E5/24</f>
         <v>45208.385416666664</v>
       </c>
-      <c r="G5" s="20">
+      <c r="G5" s="18">
         <v>25</v>
       </c>
-      <c r="H5" s="28" t="s">
+      <c r="H5" s="24" t="s">
         <v>13</v>
       </c>
       <c r="I5" s="2" t="s">
@@ -3274,25 +3274,25 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="31" t="str">
+      <c r="B6" s="27" t="str">
         <f>_xlfn.CONCAT(B5,",",C5,",",D6,",",F6,",",I5,",",J5)</f>
         <v>212,I212,1696756500,1696842900,BOM,TYO</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="17">
         <f>(D5-25569)*86400</f>
         <v>1696756499.9999998</v>
       </c>
-      <c r="F6" s="19">
+      <c r="F6" s="17">
         <f>(F5-25569)*86400</f>
         <v>1696842899.9999998</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="12">
         <f>G5*1000000000000000000</f>
         <v>2.5E+19</v>
       </c>
@@ -3301,7 +3301,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="10" t="s">
         <v>30</v>
       </c>
       <c r="D7" s="4">
@@ -3319,76 +3319,76 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="D10" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="26"/>
-      <c r="F10" s="5" t="s">
+      <c r="E10" s="32"/>
+      <c r="F10" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5" t="s">
+      <c r="G10" s="33"/>
+      <c r="H10" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="I10" s="5"/>
+      <c r="I10" s="33"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B11" s="10"/>
-      <c r="C11" s="7" t="s">
+      <c r="B11" s="34"/>
+      <c r="C11" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="24" t="s">
+      <c r="D11" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="23" t="s">
+      <c r="E11" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="I11" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="7">
         <v>1</v>
       </c>
-      <c r="D12" s="27" t="s">
+      <c r="D12" s="23" t="s">
         <v>26</v>
       </c>
       <c r="E12" s="3">
         <f>$D$6-(24*($C$2))</f>
         <v>1696755059.9999998</v>
       </c>
-      <c r="F12" s="34" t="str">
+      <c r="F12" s="30" t="str">
         <f>IFERROR((D12/86400)+DATE(1970,1,1),_xlfn.CONCAT("Before ==&gt;"))</f>
         <v>Before ==&gt;</v>
       </c>
-      <c r="G12" s="34">
-        <f t="shared" ref="G12:G15" si="0">IFERROR((E12/86400)+DATE(1970,1,1),"&lt;== After")</f>
+      <c r="G12" s="30">
+        <f t="shared" ref="G12:G14" si="0">IFERROR((E12/86400)+DATE(1970,1,1),"&lt;== After")</f>
         <v>45207.368749999994</v>
       </c>
-      <c r="H12" s="13">
+      <c r="H12" s="11">
         <f>IFERROR($G$5*C12,"--")</f>
         <v>25</v>
       </c>
-      <c r="I12" s="13">
+      <c r="I12" s="11">
         <f>IFERROR($G$5*C12,"--")</f>
         <v>25</v>
       </c>
@@ -3397,10 +3397,10 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="7">
         <v>0.8</v>
       </c>
       <c r="D13" s="3">
@@ -3411,19 +3411,19 @@
         <f>+D13+(20*$C$2)-1</f>
         <v>1696756259.9999998</v>
       </c>
-      <c r="F13" s="34">
+      <c r="F13" s="30">
         <f t="shared" ref="F13:F15" si="1">IFERROR((D13/86400)+DATE(1970,1,1),_xlfn.CONCAT("Before ==&gt;"))</f>
         <v>45207.368761574071</v>
       </c>
-      <c r="G13" s="34">
+      <c r="G13" s="30">
         <f t="shared" si="0"/>
         <v>45207.382638888885</v>
       </c>
-      <c r="H13" s="13">
+      <c r="H13" s="11">
         <f>IFERROR($G$5*C13,"--")</f>
         <v>20</v>
       </c>
-      <c r="I13" s="13">
+      <c r="I13" s="11">
         <f>IFERROR($G$5*C13,"--")</f>
         <v>20</v>
       </c>
@@ -3432,10 +3432,10 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="7">
         <v>0.4</v>
       </c>
       <c r="D14" s="3">
@@ -3446,19 +3446,19 @@
         <f>+D14+(2*$C$2)-1</f>
         <v>1696756379.9999998</v>
       </c>
-      <c r="F14" s="34">
+      <c r="F14" s="30">
         <f t="shared" si="1"/>
         <v>45207.382650462961</v>
       </c>
-      <c r="G14" s="34">
+      <c r="G14" s="30">
         <f t="shared" si="0"/>
         <v>45207.384027777778</v>
       </c>
-      <c r="H14" s="13">
+      <c r="H14" s="11">
         <f>IFERROR($G$5*C14,"--")</f>
         <v>10</v>
       </c>
-      <c r="I14" s="13">
+      <c r="I14" s="11">
         <f>IFERROR($G$5*C14,"--")</f>
         <v>10</v>
       </c>
@@ -3467,32 +3467,32 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="9" t="s">
         <v>27</v>
       </c>
       <c r="D15" s="3">
         <f>E14+1</f>
         <v>1696756380.9999998</v>
       </c>
-      <c r="E15" s="27" t="s">
+      <c r="E15" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="F15" s="34">
+      <c r="F15" s="30">
         <f t="shared" si="1"/>
         <v>45207.384039351848</v>
       </c>
-      <c r="G15" s="34" t="str">
+      <c r="G15" s="30" t="str">
         <f>IFERROR((E15/86400)+DATE(1970,1,1),"&lt;== After")</f>
         <v>&lt;== After</v>
       </c>
-      <c r="H15" s="13" t="str">
+      <c r="H15" s="11" t="str">
         <f>IFERROR($G$5*C15,"--")</f>
         <v>--</v>
       </c>
-      <c r="I15" s="13" t="str">
+      <c r="I15" s="11" t="str">
         <f>IFERROR($G$5*C15,"--")</f>
         <v>--</v>
       </c>
@@ -3506,76 +3506,76 @@
       </c>
     </row>
     <row r="19" spans="2:10" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D19" s="25" t="s">
+      <c r="D19" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="26"/>
-      <c r="F19" s="5" t="s">
+      <c r="E19" s="32"/>
+      <c r="F19" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5" t="s">
+      <c r="G19" s="33"/>
+      <c r="H19" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="I19" s="5"/>
+      <c r="I19" s="33"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B20" s="10"/>
-      <c r="C20" s="7" t="s">
+      <c r="B20" s="34"/>
+      <c r="C20" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D20" s="24" t="s">
+      <c r="D20" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="E20" s="23" t="s">
+      <c r="E20" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G20" s="6" t="s">
+      <c r="G20" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="H20" s="6" t="s">
+      <c r="H20" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I20" s="6" t="s">
+      <c r="I20" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="8">
+      <c r="C21" s="7">
         <v>0</v>
       </c>
-      <c r="D21" s="27" t="s">
+      <c r="D21" s="23" t="s">
         <v>26</v>
       </c>
       <c r="E21" s="3">
         <f>$D$6+(2*($C$2))-1</f>
         <v>1696756618.9999998</v>
       </c>
-      <c r="F21" s="34" t="str">
+      <c r="F21" s="30" t="str">
         <f t="shared" ref="F21:F25" si="2">IFERROR((D21/86400)+DATE(1970,1,1),_xlfn.CONCAT("Before ==&gt;"))</f>
         <v>Before ==&gt;</v>
       </c>
-      <c r="G21" s="34">
+      <c r="G21" s="30">
         <f t="shared" ref="G21:G25" si="3">IFERROR((E21/86400)+DATE(1970,1,1),"&lt;== After")</f>
         <v>45207.386793981481</v>
       </c>
-      <c r="H21" s="13">
+      <c r="H21" s="11">
         <f>+$G$5*C21</f>
         <v>0</v>
       </c>
-      <c r="I21" s="13">
+      <c r="I21" s="11">
         <f>$G$5-H21</f>
         <v>25</v>
       </c>
@@ -3584,10 +3584,10 @@
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="8">
+      <c r="C22" s="7">
         <v>0.1</v>
       </c>
       <c r="D22" s="3">
@@ -3598,19 +3598,19 @@
         <f>+D22+(10*$C$2)-1</f>
         <v>1696757218.9999998</v>
       </c>
-      <c r="F22" s="34">
+      <c r="F22" s="30">
         <f t="shared" si="2"/>
         <v>45207.38680555555</v>
       </c>
-      <c r="G22" s="34">
+      <c r="G22" s="30">
         <f t="shared" si="3"/>
         <v>45207.393738425919</v>
       </c>
-      <c r="H22" s="13">
+      <c r="H22" s="11">
         <f>+$G$5*C22</f>
         <v>2.5</v>
       </c>
-      <c r="I22" s="13">
+      <c r="I22" s="11">
         <f>$G$5-H22</f>
         <v>22.5</v>
       </c>
@@ -3619,10 +3619,10 @@
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="8">
+      <c r="C23" s="7">
         <v>0.4</v>
       </c>
       <c r="D23" s="3">
@@ -3633,19 +3633,19 @@
         <f>+D23+(10*$C$2)-1</f>
         <v>1696757818.9999998</v>
       </c>
-      <c r="F23" s="34">
+      <c r="F23" s="30">
         <f t="shared" si="2"/>
         <v>45207.393749999996</v>
       </c>
-      <c r="G23" s="34">
+      <c r="G23" s="30">
         <f t="shared" si="3"/>
         <v>45207.400682870371</v>
       </c>
-      <c r="H23" s="13">
+      <c r="H23" s="11">
         <f>+$G$5*C23</f>
         <v>10</v>
       </c>
-      <c r="I23" s="13">
+      <c r="I23" s="11">
         <f>$G$5-H23</f>
         <v>15</v>
       </c>
@@ -3654,32 +3654,32 @@
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C24" s="8">
+      <c r="C24" s="7">
         <v>1</v>
       </c>
       <c r="D24" s="3">
         <f>+E23+1</f>
         <v>1696757819.9999998</v>
       </c>
-      <c r="E24" s="27" t="s">
+      <c r="E24" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="F24" s="34">
+      <c r="F24" s="30">
         <f t="shared" si="2"/>
         <v>45207.400694444441</v>
       </c>
-      <c r="G24" s="34" t="str">
+      <c r="G24" s="30" t="str">
         <f t="shared" si="3"/>
         <v>&lt;== After</v>
       </c>
-      <c r="H24" s="13">
+      <c r="H24" s="11">
         <f>+$G$5*C24</f>
         <v>25</v>
       </c>
-      <c r="I24" s="13">
+      <c r="I24" s="11">
         <f>$G$5-H24</f>
         <v>0</v>
       </c>
@@ -3688,10 +3688,10 @@
       </c>
     </row>
     <row r="25" spans="2:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="8">
+      <c r="C25" s="7">
         <v>1</v>
       </c>
       <c r="D25" s="3">
@@ -3702,19 +3702,19 @@
         <f>$D$6-1</f>
         <v>1696756498.9999998</v>
       </c>
-      <c r="F25" s="34">
+      <c r="F25" s="30">
         <f t="shared" si="2"/>
         <v>45207.368749999994</v>
       </c>
-      <c r="G25" s="34">
+      <c r="G25" s="30">
         <f t="shared" si="3"/>
         <v>45207.385405092587</v>
       </c>
-      <c r="H25" s="13">
+      <c r="H25" s="11">
         <f>+$G$5*C25</f>
         <v>25</v>
       </c>
-      <c r="I25" s="13">
+      <c r="I25" s="11">
         <f>$G$5-H25</f>
         <v>0</v>
       </c>
@@ -3766,34 +3766,34 @@
       <c r="C1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="15">
+      <c r="D1" s="13">
         <v>60</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="13" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C2" s="16">
+      <c r="C2" s="14">
         <f>D1</f>
         <v>60</v>
       </c>
-      <c r="D2" s="17">
+      <c r="D2" s="15">
         <f>+D1*60</f>
         <v>3600</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="15" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="10" t="s">
         <v>28</v>
       </c>
       <c r="C3" s="2"/>
@@ -3801,31 +3801,31 @@
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="29" t="s">
+      <c r="E4" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="30" t="s">
+      <c r="G4" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="21" t="s">
+      <c r="H4" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="I4" s="21" t="s">
+      <c r="I4" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="J4" s="21" t="s">
+      <c r="J4" s="19" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3833,24 +3833,24 @@
       <c r="B5" s="3">
         <v>223</v>
       </c>
-      <c r="C5" s="32" t="str">
+      <c r="C5" s="28" t="str">
         <f>_xlfn.CONCAT("I",B5)</f>
         <v>I223</v>
       </c>
-      <c r="D5" s="33">
+      <c r="D5" s="29">
         <v>45207.375</v>
       </c>
       <c r="E5" s="2">
         <v>24</v>
       </c>
-      <c r="F5" s="33">
+      <c r="F5" s="29">
         <f>D5+E5/24</f>
         <v>45208.375</v>
       </c>
-      <c r="G5" s="20">
+      <c r="G5" s="18">
         <v>25</v>
       </c>
-      <c r="H5" s="28" t="s">
+      <c r="H5" s="24" t="s">
         <v>13</v>
       </c>
       <c r="I5" s="2" t="s">
@@ -3861,25 +3861,25 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="31" t="str">
+      <c r="B6" s="27" t="str">
         <f>_xlfn.CONCAT(B5,",",C5,",",D6,",",F6,",",I5,",",J5)</f>
         <v>223,I223,1696755600,1696842000,BOM,SYD</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="17">
         <f>(D5-25569)*86400</f>
         <v>1696755600</v>
       </c>
-      <c r="F6" s="19">
+      <c r="F6" s="17">
         <f>(F5-25569)*86400</f>
         <v>1696842000</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="12">
         <f>G5*1000000000000000000</f>
         <v>2.5E+19</v>
       </c>
@@ -3888,7 +3888,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="10" t="s">
         <v>30</v>
       </c>
       <c r="D7" s="4">
@@ -3906,76 +3906,76 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="D10" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="26"/>
-      <c r="F10" s="5" t="s">
+      <c r="E10" s="32"/>
+      <c r="F10" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5" t="s">
+      <c r="G10" s="33"/>
+      <c r="H10" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="I10" s="5"/>
+      <c r="I10" s="33"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B11" s="10"/>
-      <c r="C11" s="7" t="s">
+      <c r="B11" s="34"/>
+      <c r="C11" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="24" t="s">
+      <c r="D11" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="23" t="s">
+      <c r="E11" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="I11" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="7">
         <v>1</v>
       </c>
-      <c r="D12" s="27" t="s">
+      <c r="D12" s="23" t="s">
         <v>26</v>
       </c>
       <c r="E12" s="3">
         <f>$D$6-(24*($C$2))</f>
         <v>1696754160</v>
       </c>
-      <c r="F12" s="34" t="str">
+      <c r="F12" s="30" t="str">
         <f>IFERROR((D12/86400)+DATE(1970,1,1),_xlfn.CONCAT("Before ==&gt;"))</f>
         <v>Before ==&gt;</v>
       </c>
-      <c r="G12" s="34">
-        <f t="shared" ref="G12:G15" si="0">IFERROR((E12/86400)+DATE(1970,1,1),"&lt;== After")</f>
+      <c r="G12" s="30">
+        <f t="shared" ref="G12:G14" si="0">IFERROR((E12/86400)+DATE(1970,1,1),"&lt;== After")</f>
         <v>45207.358333333337</v>
       </c>
-      <c r="H12" s="13">
+      <c r="H12" s="11">
         <f>IFERROR($G$5*C12,"--")</f>
         <v>25</v>
       </c>
-      <c r="I12" s="13">
+      <c r="I12" s="11">
         <f>IFERROR($G$5*C12,"--")</f>
         <v>25</v>
       </c>
@@ -3984,10 +3984,10 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="7">
         <v>0.8</v>
       </c>
       <c r="D13" s="3">
@@ -3998,19 +3998,19 @@
         <f>+D13+(20*$C$2)-1</f>
         <v>1696755360</v>
       </c>
-      <c r="F13" s="34">
+      <c r="F13" s="30">
         <f t="shared" ref="F13:F15" si="1">IFERROR((D13/86400)+DATE(1970,1,1),_xlfn.CONCAT("Before ==&gt;"))</f>
         <v>45207.358344907407</v>
       </c>
-      <c r="G13" s="34">
+      <c r="G13" s="30">
         <f t="shared" si="0"/>
         <v>45207.37222222222</v>
       </c>
-      <c r="H13" s="13">
+      <c r="H13" s="11">
         <f>IFERROR($G$5*C13,"--")</f>
         <v>20</v>
       </c>
-      <c r="I13" s="13">
+      <c r="I13" s="11">
         <f>IFERROR($G$5*C13,"--")</f>
         <v>20</v>
       </c>
@@ -4019,10 +4019,10 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="7">
         <v>0.4</v>
       </c>
       <c r="D14" s="3">
@@ -4033,19 +4033,19 @@
         <f>+D14+(2*$C$2)-1</f>
         <v>1696755480</v>
       </c>
-      <c r="F14" s="34">
+      <c r="F14" s="30">
         <f t="shared" si="1"/>
         <v>45207.372233796297</v>
       </c>
-      <c r="G14" s="34">
+      <c r="G14" s="30">
         <f t="shared" si="0"/>
         <v>45207.373611111107</v>
       </c>
-      <c r="H14" s="13">
+      <c r="H14" s="11">
         <f>IFERROR($G$5*C14,"--")</f>
         <v>10</v>
       </c>
-      <c r="I14" s="13">
+      <c r="I14" s="11">
         <f>IFERROR($G$5*C14,"--")</f>
         <v>10</v>
       </c>
@@ -4054,32 +4054,32 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="9" t="s">
         <v>27</v>
       </c>
       <c r="D15" s="3">
         <f>E14+1</f>
         <v>1696755481</v>
       </c>
-      <c r="E15" s="27" t="s">
+      <c r="E15" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="F15" s="34">
+      <c r="F15" s="30">
         <f t="shared" si="1"/>
         <v>45207.373622685191</v>
       </c>
-      <c r="G15" s="34" t="str">
+      <c r="G15" s="30" t="str">
         <f>IFERROR((E15/86400)+DATE(1970,1,1),"&lt;== After")</f>
         <v>&lt;== After</v>
       </c>
-      <c r="H15" s="13" t="str">
+      <c r="H15" s="11" t="str">
         <f>IFERROR($G$5*C15,"--")</f>
         <v>--</v>
       </c>
-      <c r="I15" s="13" t="str">
+      <c r="I15" s="11" t="str">
         <f>IFERROR($G$5*C15,"--")</f>
         <v>--</v>
       </c>
@@ -4093,76 +4093,76 @@
       </c>
     </row>
     <row r="19" spans="2:10" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D19" s="25" t="s">
+      <c r="D19" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="26"/>
-      <c r="F19" s="5" t="s">
+      <c r="E19" s="32"/>
+      <c r="F19" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5" t="s">
+      <c r="G19" s="33"/>
+      <c r="H19" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="I19" s="5"/>
+      <c r="I19" s="33"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B20" s="10"/>
-      <c r="C20" s="7" t="s">
+      <c r="B20" s="34"/>
+      <c r="C20" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D20" s="24" t="s">
+      <c r="D20" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="E20" s="23" t="s">
+      <c r="E20" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G20" s="6" t="s">
+      <c r="G20" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="H20" s="6" t="s">
+      <c r="H20" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I20" s="6" t="s">
+      <c r="I20" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="8">
+      <c r="C21" s="7">
         <v>0</v>
       </c>
-      <c r="D21" s="27" t="s">
+      <c r="D21" s="23" t="s">
         <v>26</v>
       </c>
       <c r="E21" s="3">
         <f>$D$6+(2*($C$2))-1</f>
         <v>1696755719</v>
       </c>
-      <c r="F21" s="34" t="str">
+      <c r="F21" s="30" t="str">
         <f t="shared" ref="F21:F25" si="2">IFERROR((D21/86400)+DATE(1970,1,1),_xlfn.CONCAT("Before ==&gt;"))</f>
         <v>Before ==&gt;</v>
       </c>
-      <c r="G21" s="34">
+      <c r="G21" s="30">
         <f t="shared" ref="G21:G25" si="3">IFERROR((E21/86400)+DATE(1970,1,1),"&lt;== After")</f>
         <v>45207.376377314809</v>
       </c>
-      <c r="H21" s="13">
+      <c r="H21" s="11">
         <f>+$G$5*C21</f>
         <v>0</v>
       </c>
-      <c r="I21" s="13">
+      <c r="I21" s="11">
         <f>$G$5-H21</f>
         <v>25</v>
       </c>
@@ -4171,10 +4171,10 @@
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="8">
+      <c r="C22" s="7">
         <v>0.1</v>
       </c>
       <c r="D22" s="3">
@@ -4185,19 +4185,19 @@
         <f>+D22+(10*$C$2)-1</f>
         <v>1696756319</v>
       </c>
-      <c r="F22" s="34">
+      <c r="F22" s="30">
         <f t="shared" si="2"/>
         <v>45207.376388888893</v>
       </c>
-      <c r="G22" s="34">
+      <c r="G22" s="30">
         <f t="shared" si="3"/>
         <v>45207.383321759262</v>
       </c>
-      <c r="H22" s="13">
+      <c r="H22" s="11">
         <f>+$G$5*C22</f>
         <v>2.5</v>
       </c>
-      <c r="I22" s="13">
+      <c r="I22" s="11">
         <f>$G$5-H22</f>
         <v>22.5</v>
       </c>
@@ -4206,10 +4206,10 @@
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="8">
+      <c r="C23" s="7">
         <v>0.4</v>
       </c>
       <c r="D23" s="3">
@@ -4220,19 +4220,19 @@
         <f>+D23+(10*$C$2)-1</f>
         <v>1696756919</v>
       </c>
-      <c r="F23" s="34">
+      <c r="F23" s="30">
         <f t="shared" si="2"/>
         <v>45207.383333333331</v>
       </c>
-      <c r="G23" s="34">
+      <c r="G23" s="30">
         <f t="shared" si="3"/>
         <v>45207.3902662037</v>
       </c>
-      <c r="H23" s="13">
+      <c r="H23" s="11">
         <f>+$G$5*C23</f>
         <v>10</v>
       </c>
-      <c r="I23" s="13">
+      <c r="I23" s="11">
         <f>$G$5-H23</f>
         <v>15</v>
       </c>
@@ -4241,32 +4241,32 @@
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C24" s="8">
+      <c r="C24" s="7">
         <v>1</v>
       </c>
       <c r="D24" s="3">
         <f>+E23+1</f>
         <v>1696756920</v>
       </c>
-      <c r="E24" s="27" t="s">
+      <c r="E24" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="F24" s="34">
+      <c r="F24" s="30">
         <f t="shared" si="2"/>
         <v>45207.390277777777</v>
       </c>
-      <c r="G24" s="34" t="str">
+      <c r="G24" s="30" t="str">
         <f t="shared" si="3"/>
         <v>&lt;== After</v>
       </c>
-      <c r="H24" s="13">
+      <c r="H24" s="11">
         <f>+$G$5*C24</f>
         <v>25</v>
       </c>
-      <c r="I24" s="13">
+      <c r="I24" s="11">
         <f>$G$5-H24</f>
         <v>0</v>
       </c>
@@ -4275,10 +4275,10 @@
       </c>
     </row>
     <row r="25" spans="2:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="8">
+      <c r="C25" s="7">
         <v>1</v>
       </c>
       <c r="D25" s="3">
@@ -4289,19 +4289,19 @@
         <f>$D$6-1</f>
         <v>1696755599</v>
       </c>
-      <c r="F25" s="34">
+      <c r="F25" s="30">
         <f t="shared" si="2"/>
         <v>45207.358333333337</v>
       </c>
-      <c r="G25" s="34">
+      <c r="G25" s="30">
         <f t="shared" si="3"/>
         <v>45207.37498842593</v>
       </c>
-      <c r="H25" s="13">
+      <c r="H25" s="11">
         <f>+$G$5*C25</f>
         <v>25</v>
       </c>
-      <c r="I25" s="13">
+      <c r="I25" s="11">
         <f>$G$5-H25</f>
         <v>0</v>
       </c>

</xml_diff>